<commit_message>
Final paper and oral presentation submitted 2
</commit_message>
<xml_diff>
--- a/Written Assignment 2/Didrik Wiig-Andersen - CLST1201 - Data from Papyri.xlsx
+++ b/Written Assignment 2/Didrik Wiig-Andersen - CLST1201 - Data from Papyri.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1544" documentId="8_{556D77AE-52DF-7443-BABD-8F9020596E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{776E0DF1-B3AA-DA49-BC52-93FA5FF8CAEE}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="2520" windowWidth="30240" windowHeight="18900" xr2:uid="{AFB80346-FCA0-8141-8D51-87A7F0CD1C9A}"/>
+    <workbookView xWindow="51200" yWindow="2540" windowWidth="30240" windowHeight="17420" xr2:uid="{AFB80346-FCA0-8141-8D51-87A7F0CD1C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="353 hits, April 1 2025" sheetId="1" r:id="rId1"/>
@@ -1459,8 +1459,8 @@
   <dimension ref="A1:S252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A253" sqref="A253"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>